<commit_message>
updated the schedule... hopeless anyway
</commit_message>
<xml_diff>
--- a/planning.xlsx
+++ b/planning.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="23820" windowHeight="9855"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="15240" windowHeight="7965"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="6">
   <si>
     <t>Project</t>
   </si>
@@ -29,6 +29,12 @@
   <si>
     <t>x</t>
   </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>Rette</t>
+  </si>
 </sst>
 </file>
 
@@ -43,12 +49,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -63,8 +75,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -366,41 +379,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:L10"/>
+  <dimension ref="C1:Q11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="E1">
-        <v>45</v>
-      </c>
+    <row r="1" spans="3:17" x14ac:dyDescent="0.25">
       <c r="F1">
         <v>46</v>
       </c>
       <c r="G1">
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="H1">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="I1">
-        <v>49</v>
+        <v>20</v>
       </c>
       <c r="J1">
-        <v>50</v>
+        <v>21</v>
       </c>
       <c r="K1">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="L1">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="3:12" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="M1">
+        <v>24</v>
+      </c>
+      <c r="N1">
+        <v>25</v>
+      </c>
+      <c r="O1">
+        <v>26</v>
+      </c>
+      <c r="P1">
+        <v>27</v>
+      </c>
+      <c r="Q1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C2">
         <v>1</v>
       </c>
@@ -408,7 +433,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C3">
         <v>2</v>
       </c>
@@ -416,7 +441,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C4">
         <v>3</v>
       </c>
@@ -426,8 +451,10 @@
       <c r="E4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+    </row>
+    <row r="5" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C5">
         <v>4</v>
       </c>
@@ -437,43 +464,80 @@
       <c r="E5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>4</v>
+      </c>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+    </row>
+    <row r="6" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>5</v>
       </c>
       <c r="F6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>4</v>
+      </c>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+    </row>
+    <row r="7" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>6</v>
       </c>
-      <c r="G7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="H7" t="s">
+        <v>3</v>
+      </c>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+    </row>
+    <row r="8" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C8">
         <v>7</v>
       </c>
       <c r="H8" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+    </row>
+    <row r="9" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>9</v>
+      </c>
+      <c r="I9" t="s">
+        <v>3</v>
+      </c>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+    </row>
+    <row r="10" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>0</v>
       </c>
       <c r="I10" t="s">
         <v>3</v>
       </c>
-      <c r="J10" t="s">
-        <v>3</v>
-      </c>
       <c r="K10" t="s">
         <v>3</v>
+      </c>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" t="s">
+        <v>3</v>
+      </c>
+      <c r="O10" t="s">
+        <v>3</v>
+      </c>
+      <c r="P10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>